<commit_message>
Updated to work for PrintedCircuitBoard
</commit_message>
<xml_diff>
--- a/data/PrintedCircuitBoard/BOM_1.xlsx
+++ b/data/PrintedCircuitBoard/BOM_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wingwers\LCAproductsystemassembly_resources\data\PrintedCircuitBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesle\LCAproductsystemassembly_resources\data\PrintedCircuitBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17842B57-177D-4108-9A47-68A563670B5F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9CDD57-9438-4BC4-8175-45E72C5A7CB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="22" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <definedName name="_DAT7">#REF!</definedName>
     <definedName name="_DAT8">#REF!</definedName>
     <definedName name="_DAT9">#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$F$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$F$9</definedName>
     <definedName name="AutoFormatting">TRUE</definedName>
     <definedName name="cancellocation">#REF!</definedName>
     <definedName name="CPN_vendor">#REF!</definedName>
@@ -68,13 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="24">
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>1206 Chip Resistor or Capacitor</t>
   </si>
@@ -164,6 +158,12 @@
   </si>
   <si>
     <t>Board</t>
+  </si>
+  <si>
+    <t>QNA</t>
+  </si>
+  <si>
+    <t>Part Name</t>
   </si>
 </sst>
 </file>
@@ -3013,7 +3013,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3057,6 +3057,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="502" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="46" borderId="17" xfId="502" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4130,11 +4133,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75"/>
@@ -4150,22 +4153,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4173,14 +4176,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12">
         <v>1</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2" s="6"/>
     </row>
@@ -4189,17 +4192,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -4211,13 +4214,13 @@
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -4225,17 +4228,17 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4243,17 +4246,17 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4261,17 +4264,17 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -4279,17 +4282,17 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -4297,362 +4300,110 @@
         <v>1</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="4">
         <v>1</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="B10" s="7"/>
       <c r="C10" s="13"/>
       <c r="D10" s="5">
         <v>1</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="4">
         <v>1</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="13"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="5">
         <v>1</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>6</v>
+      <c r="E11" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="4">
         <v>1</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="13"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="5">
         <v>1</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>6</v>
+      <c r="E12" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="4">
         <v>1</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="13"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="5">
         <v>1</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>6</v>
+      <c r="E13" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="4">
         <v>1</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="13"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="5">
         <v>1</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>6</v>
+      <c r="E14" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="4">
-        <v>1</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="5">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="4">
-        <v>1</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="5">
-        <v>1</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4">
-        <v>1</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="5">
-        <v>1</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="4">
-        <v>1</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="5">
-        <v>1</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="4">
-        <v>1</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="5">
-        <v>1</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="4">
-        <v>1</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="5">
-        <v>1</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="4">
-        <v>1</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="5">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="4">
-        <v>1</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="5">
-        <v>1</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="4">
-        <v>1</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="5">
-        <v>1</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="4">
-        <v>1</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="5">
-        <v>1</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="4">
-        <v>1</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="5">
-        <v>1</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="4">
-        <v>1</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="5">
-        <v>1</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="4">
-        <v>1</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="5">
-        <v>1</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="4">
-        <v>1</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="5">
-        <v>1</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
@@ -4672,8 +4423,44 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <Records_x0020_Status xmlns="d73cf8ff-ef45-492d-adb8-ac72f7aa27c7">Pending</Records_x0020_Status>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2019-11-01T22:30:29+00:00</Document_x0020_Creation_x0020_Date>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <Records_x0020_Date xmlns="d73cf8ff-ef45-492d-adb8-ac72f7aa27c7" xsi:nil="true"/>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5126,44 +4913,8 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <Records_x0020_Status xmlns="d73cf8ff-ef45-492d-adb8-ac72f7aa27c7">Pending</Records_x0020_Status>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2019-11-01T22:30:29+00:00</Document_x0020_Creation_x0020_Date>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <Records_x0020_Date xmlns="d73cf8ff-ef45-492d-adb8-ac72f7aa27c7" xsi:nil="true"/>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5175,9 +4926,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4927B198-0C86-471F-8E9C-6F8FE35F534B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4863E34D-07FE-4D95-8156-AC9E07DA48AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="53e29f70-1d13-4545-912f-f1092da9a3f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="d73cf8ff-ef45-492d-adb8-ac72f7aa27c7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5206,22 +4970,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4863E34D-07FE-4D95-8156-AC9E07DA48AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4927B198-0C86-471F-8E9C-6F8FE35F534B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="53e29f70-1d13-4545-912f-f1092da9a3f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="d73cf8ff-ef45-492d-adb8-ac72f7aa27c7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>